<commit_message>
updated control flow signals on the signal sheet
</commit_message>
<xml_diff>
--- a/Proj2_control_signals (1).xlsx
+++ b/Proj2_control_signals (1).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\my.files.iastate.edu\Users\adto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cpre381\Proj2\Proj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="705" yWindow="465" windowWidth="27720" windowHeight="17040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Instruction</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>Control Signals</t>
-  </si>
-  <si>
-    <t>Note: these are example control signals from the text and your skeleton code; you will need to add more control signals; you may rename any control signals, except those given in the skeleton code.</t>
-  </si>
-  <si>
-    <t>Note: other signals you may have must be correctly assigned for the add; if you redefined these signals, you probably will need to change the sample values</t>
   </si>
   <si>
     <t>addi</t>
@@ -334,6 +328,42 @@
   </si>
   <si>
     <t>"1110"</t>
+  </si>
+  <si>
+    <t>s_SignExt[sign or unsign extend imm]</t>
+  </si>
+  <si>
+    <t>s_UnsignIns[do not set overflow for unsigned instructions</t>
+  </si>
+  <si>
+    <t>s_j</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>beq</t>
+  </si>
+  <si>
+    <t>"000010"</t>
+  </si>
+  <si>
+    <t>"000100"</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>"----"</t>
+  </si>
+  <si>
+    <t>s_jr</t>
+  </si>
+  <si>
+    <t>s_Branch</t>
   </si>
 </sst>
 </file>
@@ -377,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,7 +416,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,13 +744,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -730,116 +763,142 @@
     <col min="6" max="6" width="32.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" style="4" customWidth="1"/>
+    <col min="9" max="9" width="27" style="3" customWidth="1"/>
     <col min="10" max="10" width="45.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="1"/>
+    <col min="11" max="11" width="30.75" style="4" customWidth="1"/>
+    <col min="12" max="12" width="48.375" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>53</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>7</v>
+      <c r="K2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>8</v>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -850,28 +909,43 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -882,19 +956,34 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0</v>
       </c>
       <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>100001</v>
@@ -903,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -914,19 +1003,34 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>1</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>100100</v>
@@ -935,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -946,28 +1050,43 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>0</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -978,28 +1097,43 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1010,28 +1144,43 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -1042,19 +1191,34 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>1</v>
       </c>
       <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1">
         <v>100111</v>
@@ -1063,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1074,19 +1238,34 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>0</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>100110</v>
@@ -1095,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1106,28 +1285,43 @@
       <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1138,19 +1332,34 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>0</v>
       </c>
       <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1">
         <v>100101</v>
@@ -1159,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1170,28 +1379,43 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" s="1">
         <v>1</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1202,19 +1426,34 @@
       <c r="H15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1">
         <v>101010</v>
@@ -1223,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1234,83 +1473,128 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>0</v>
       </c>
       <c r="J16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1">
         <v>101011</v>
@@ -1318,8 +1602,8 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>64</v>
+      <c r="E19" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1330,19 +1614,34 @@
       <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>0</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+      <c r="O19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -1350,8 +1649,8 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>59</v>
+      <c r="E20" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1362,19 +1661,34 @@
       <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>0</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1">
         <v>10</v>
@@ -1383,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1394,19 +1708,34 @@
       <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1">
         <v>11</v>
@@ -1415,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1426,31 +1755,46 @@
       <c r="H22" s="1">
         <v>1</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>0</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
@@ -1458,19 +1802,34 @@
       <c r="H23" s="1">
         <v>0</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+      <c r="O23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C24" s="1">
         <v>100011</v>
@@ -1479,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1490,10 +1849,166 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <v>0</v>
       </c>
       <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>